<commit_message>
Equipment and User Uploading Works
</commit_message>
<xml_diff>
--- a/EquipmentUploadFormat.xlsx
+++ b/EquipmentUploadFormat.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathaniel Angelico\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathaniel Angelico\Desktop\ANS-SEIS-TV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A82136-13F8-4122-8C19-E30D55F14A1F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51818B17-1CC5-4A7C-BEA2-58C790FD6D33}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{BF1B3BD2-351C-4AC5-B15B-A04BFBAC4893}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>EquipmentName</t>
   </si>
@@ -39,31 +39,58 @@
     <t>EquipmentQuantity</t>
   </si>
   <si>
-    <t xml:space="preserve">TestEquipment </t>
-  </si>
-  <si>
-    <t>TestEquipment 1</t>
-  </si>
-  <si>
-    <t>TestEquipment 2</t>
-  </si>
-  <si>
-    <t>TestEquipment 3</t>
-  </si>
-  <si>
-    <t>TestEquipment 4</t>
-  </si>
-  <si>
-    <t>TestEquipment 5</t>
-  </si>
-  <si>
-    <t>Computer</t>
+    <t>Computer1</t>
+  </si>
+  <si>
+    <t>Test1</t>
   </si>
   <si>
     <t>Computer2</t>
   </si>
   <si>
-    <t>Computer23</t>
+    <t>Computer3</t>
+  </si>
+  <si>
+    <t>Computer4</t>
+  </si>
+  <si>
+    <t>Computer5</t>
+  </si>
+  <si>
+    <t>Computer6</t>
+  </si>
+  <si>
+    <t>Computer7</t>
+  </si>
+  <si>
+    <t>Computer8</t>
+  </si>
+  <si>
+    <t>Computer9</t>
+  </si>
+  <si>
+    <t>Test2</t>
+  </si>
+  <si>
+    <t>Test3</t>
+  </si>
+  <si>
+    <t>Test4</t>
+  </si>
+  <si>
+    <t>Test5</t>
+  </si>
+  <si>
+    <t>Test6</t>
+  </si>
+  <si>
+    <t>Test7</t>
+  </si>
+  <si>
+    <t>Test8</t>
+  </si>
+  <si>
+    <t>Test9</t>
   </si>
 </sst>
 </file>
@@ -421,7 +448,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,125 +476,125 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C3">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C5">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C6">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C7">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C8">
         <v>200</v>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C9">
         <v>200</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C10">
         <v>200</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>